<commit_message>
Prefetch closing price data for all stocks and dates to reduce computation time [fix #5]
</commit_message>
<xml_diff>
--- a/multibeggar/tests/output/test_transactions_list_small_daywise_full_portfolio.xlsx
+++ b/multibeggar/tests/output/test_transactions_list_small_daywise_full_portfolio.xlsx
@@ -501,7 +501,7 @@
         <v>395.9999847412109</v>
       </c>
       <c r="H2" t="n">
-        <v>0.2024602832988485</v>
+        <v>0.2020408164059704</v>
       </c>
     </row>
     <row r="3">
@@ -525,13 +525,13 @@
         </is>
       </c>
       <c r="F3" t="n">
-        <v>77.99695587158203</v>
+        <v>78.19999694824219</v>
       </c>
       <c r="G3" t="n">
-        <v>1559.939117431641</v>
+        <v>1563.999938964844</v>
       </c>
       <c r="H3" t="n">
-        <v>0.7975397167011515</v>
+        <v>0.7979591835940296</v>
       </c>
     </row>
     <row r="4">
@@ -621,7 +621,7 @@
         <v>795.5000305175781</v>
       </c>
       <c r="H6" t="n">
-        <v>0.327064859280383</v>
+        <v>0.3264929204294104</v>
       </c>
     </row>
     <row r="7">
@@ -645,13 +645,13 @@
         </is>
       </c>
       <c r="F7" t="n">
-        <v>81.83696746826172</v>
+        <v>82.05000305175781</v>
       </c>
       <c r="G7" t="n">
-        <v>1636.739349365234</v>
+        <v>1641.000061035156</v>
       </c>
       <c r="H7" t="n">
-        <v>0.672935140719617</v>
+        <v>0.6735070795705895</v>
       </c>
     </row>
     <row r="8">
@@ -681,7 +681,7 @@
         <v>830</v>
       </c>
       <c r="H8" t="n">
-        <v>0.1998387472810739</v>
+        <v>0.1994233483076236</v>
       </c>
     </row>
     <row r="9">
@@ -705,13 +705,13 @@
         </is>
       </c>
       <c r="F9" t="n">
-        <v>83.08371734619141</v>
+        <v>83.30000305175781</v>
       </c>
       <c r="G9" t="n">
-        <v>3323.348693847656</v>
+        <v>3332.000122070312</v>
       </c>
       <c r="H9" t="n">
-        <v>0.8001612527189261</v>
+        <v>0.8005766516923764</v>
       </c>
     </row>
     <row r="10">
@@ -741,7 +741,7 @@
         <v>1708.999938964844</v>
       </c>
       <c r="H10" t="n">
-        <v>0.29448549770074</v>
+        <v>0.2939456448799682</v>
       </c>
     </row>
     <row r="11">
@@ -765,13 +765,13 @@
         </is>
       </c>
       <c r="F11" t="n">
-        <v>81.88683319091797</v>
+        <v>82.09999847412109</v>
       </c>
       <c r="G11" t="n">
-        <v>4094.341659545898</v>
+        <v>4104.999923706055</v>
       </c>
       <c r="H11" t="n">
-        <v>0.70551450229926</v>
+        <v>0.7060543551200318</v>
       </c>
     </row>
     <row r="12">
@@ -831,7 +831,7 @@
         <v>1923.000030517578</v>
       </c>
       <c r="H13" t="n">
-        <v>0.285609114310247</v>
+        <v>0.2850789511996523</v>
       </c>
     </row>
     <row r="14">
@@ -855,13 +855,13 @@
         </is>
       </c>
       <c r="F14" t="n">
-        <v>96.19956970214844</v>
+        <v>96.44999694824219</v>
       </c>
       <c r="G14" t="n">
-        <v>4809.978485107422</v>
+        <v>4822.499847412109</v>
       </c>
       <c r="H14" t="n">
-        <v>0.714390885689753</v>
+        <v>0.7149210488003477</v>
       </c>
     </row>
     <row r="15">
@@ -891,7 +891,7 @@
         <v>1990</v>
       </c>
       <c r="H15" t="n">
-        <v>0.1899748530660442</v>
+        <v>0.1897198552766218</v>
       </c>
     </row>
     <row r="16">
@@ -915,13 +915,13 @@
         </is>
       </c>
       <c r="F16" t="n">
-        <v>108.1684112548828</v>
+        <v>108.4499969482422</v>
       </c>
       <c r="G16" t="n">
-        <v>5408.420562744141</v>
+        <v>5422.499847412109</v>
       </c>
       <c r="H16" t="n">
-        <v>0.5163135184556231</v>
+        <v>0.516962756928909</v>
       </c>
     </row>
     <row r="17">
@@ -951,7 +951,7 @@
         <v>3076.650047302246</v>
       </c>
       <c r="H17" t="n">
-        <v>0.2937116284783327</v>
+        <v>0.2933173877944692</v>
       </c>
     </row>
     <row r="18">
@@ -981,7 +981,7 @@
         <v>2529.999923706055</v>
       </c>
       <c r="H18" t="n">
-        <v>0.1965699741749239</v>
+        <v>0.1963294899032366</v>
       </c>
     </row>
     <row r="19">
@@ -1005,13 +1005,13 @@
         </is>
       </c>
       <c r="F19" t="n">
-        <v>100.9372406005859</v>
+        <v>101.1999969482422</v>
       </c>
       <c r="G19" t="n">
-        <v>6056.234436035156</v>
+        <v>6071.999816894531</v>
       </c>
       <c r="H19" t="n">
-        <v>0.470543036596166</v>
+        <v>0.471190775767768</v>
       </c>
     </row>
     <row r="20">
@@ -1041,7 +1041,7 @@
         <v>3082.699966430664</v>
       </c>
       <c r="H20" t="n">
-        <v>0.2395123601042123</v>
+        <v>0.2392193399940886</v>
       </c>
     </row>
     <row r="21">
@@ -1071,7 +1071,7 @@
         <v>1201.800048828125</v>
       </c>
       <c r="H21" t="n">
-        <v>0.09337462912469786</v>
+        <v>0.09326039433490677</v>
       </c>
     </row>
     <row r="22">
@@ -1101,7 +1101,7 @@
         <v>3325.499954223633</v>
       </c>
       <c r="H22" t="n">
-        <v>0.2345299855249004</v>
+        <v>0.2342788964336497</v>
       </c>
     </row>
     <row r="23">
@@ -1125,13 +1125,13 @@
         </is>
       </c>
       <c r="F23" t="n">
-        <v>97.29672241210938</v>
+        <v>97.55000305175781</v>
       </c>
       <c r="G23" t="n">
-        <v>5837.803344726562</v>
+        <v>5853.000183105469</v>
       </c>
       <c r="H23" t="n">
-        <v>0.4117095031671932</v>
+        <v>0.4123393302057723</v>
       </c>
     </row>
     <row r="24">
@@ -1161,7 +1161,7 @@
         <v>3769.020080566406</v>
       </c>
       <c r="H24" t="n">
-        <v>0.2658091225698614</v>
+        <v>0.2655245458626109</v>
       </c>
     </row>
     <row r="25">
@@ -1191,7 +1191,7 @@
         <v>1247.099975585938</v>
       </c>
       <c r="H25" t="n">
-        <v>0.08795138873804499</v>
+        <v>0.08785722749796712</v>
       </c>
     </row>
     <row r="26">
@@ -1221,7 +1221,7 @@
         <v>3185.999908447266</v>
       </c>
       <c r="H26" t="n">
-        <v>0.2202929848295488</v>
+        <v>0.2200738230840038</v>
       </c>
     </row>
     <row r="27">
@@ -1245,13 +1245,13 @@
         </is>
       </c>
       <c r="F27" t="n">
-        <v>92.20995330810547</v>
+        <v>92.44999694824219</v>
       </c>
       <c r="G27" t="n">
-        <v>5532.597198486328</v>
+        <v>5546.999816894531</v>
       </c>
       <c r="H27" t="n">
-        <v>0.3825462604323004</v>
+        <v>0.3831605434493547</v>
       </c>
     </row>
     <row r="28">
@@ -1281,7 +1281,7 @@
         <v>4490.36018371582</v>
       </c>
       <c r="H28" t="n">
-        <v>0.3104817565147436</v>
+        <v>0.3101728691311063</v>
       </c>
     </row>
     <row r="29">
@@ -1311,7 +1311,7 @@
         <v>1253.599975585938</v>
       </c>
       <c r="H29" t="n">
-        <v>0.08667899822340711</v>
+        <v>0.0865927643355353</v>
       </c>
     </row>
     <row r="30">
@@ -1341,7 +1341,7 @@
         <v>3596.25</v>
       </c>
       <c r="H30" t="n">
-        <v>0.2107788414767302</v>
+        <v>0.2105908844293644</v>
       </c>
     </row>
     <row r="31">
@@ -1365,13 +1365,13 @@
         </is>
       </c>
       <c r="F31" t="n">
-        <v>97.49620056152344</v>
+        <v>97.75</v>
       </c>
       <c r="G31" t="n">
-        <v>5849.772033691406</v>
+        <v>5865</v>
       </c>
       <c r="H31" t="n">
-        <v>0.3428594152699202</v>
+        <v>0.343445404846221</v>
       </c>
     </row>
     <row r="32">
@@ -1401,7 +1401,7 @@
         <v>6373.600006103516</v>
       </c>
       <c r="H32" t="n">
-        <v>0.3735613556684267</v>
+        <v>0.3732282411635292</v>
       </c>
     </row>
     <row r="33">
@@ -1431,7 +1431,7 @@
         <v>1242.099975585938</v>
       </c>
       <c r="H33" t="n">
-        <v>0.07280038758492284</v>
+        <v>0.0727354695608855</v>
       </c>
     </row>
     <row r="34">
@@ -1551,7 +1551,7 @@
         <v>3318.000106811523</v>
       </c>
       <c r="H37" t="n">
-        <v>0.2757012999576651</v>
+        <v>0.2756603970605329</v>
       </c>
     </row>
     <row r="38">
@@ -1581,7 +1581,7 @@
         <v>6665.799713134766</v>
       </c>
       <c r="H38" t="n">
-        <v>0.5538787182061652</v>
+        <v>0.5537965450563179</v>
       </c>
     </row>
     <row r="39">
@@ -1611,7 +1611,7 @@
         <v>1365</v>
       </c>
       <c r="H39" t="n">
-        <v>0.1134214172174498</v>
+        <v>0.1134045900767662</v>
       </c>
     </row>
     <row r="40">
@@ -1635,13 +1635,13 @@
         </is>
       </c>
       <c r="F40" t="n">
-        <v>137.1928558349609</v>
+        <v>137.5500030517578</v>
       </c>
       <c r="G40" t="n">
-        <v>685.9642791748047</v>
+        <v>687.7500152587891</v>
       </c>
       <c r="H40" t="n">
-        <v>0.05699856461871995</v>
+        <v>0.05713846780638292</v>
       </c>
     </row>
     <row r="41">
@@ -1671,7 +1671,7 @@
         <v>3722.000122070312</v>
       </c>
       <c r="H41" t="n">
-        <v>0.267700449473472</v>
+        <v>0.2675888384137958</v>
       </c>
     </row>
     <row r="42">
@@ -1701,7 +1701,7 @@
         <v>6626.899719238281</v>
       </c>
       <c r="H42" t="n">
-        <v>0.4766319116800394</v>
+        <v>0.4764331918316316</v>
       </c>
     </row>
     <row r="43">
@@ -1731,7 +1731,7 @@
         <v>1327</v>
       </c>
       <c r="H43" t="n">
-        <v>0.09544290295554872</v>
+        <v>0.09540311040548617</v>
       </c>
     </row>
     <row r="44">
@@ -1755,13 +1755,13 @@
         </is>
       </c>
       <c r="F44" t="n">
-        <v>148.5133819580078</v>
+        <v>148.8999938964844</v>
       </c>
       <c r="G44" t="n">
-        <v>2227.700729370117</v>
+        <v>2233.499908447266</v>
       </c>
       <c r="H44" t="n">
-        <v>0.1602247358909399</v>
+        <v>0.1605748593490865</v>
       </c>
     </row>
     <row r="45">
@@ -1791,7 +1791,7 @@
         <v>3473.999938964844</v>
       </c>
       <c r="H45" t="n">
-        <v>0.1958556412857424</v>
+        <v>0.1957773201390204</v>
       </c>
     </row>
     <row r="46">
@@ -1821,7 +1821,7 @@
         <v>10244.2497253418</v>
       </c>
       <c r="H46" t="n">
-        <v>0.5775458073398694</v>
+        <v>0.5773148512662105</v>
       </c>
     </row>
     <row r="47">
@@ -1851,7 +1851,7 @@
         <v>1293.400024414062</v>
       </c>
       <c r="H47" t="n">
-        <v>0.07291873795947541</v>
+        <v>0.07288957832364869</v>
       </c>
     </row>
     <row r="48">
@@ -1875,13 +1875,13 @@
         </is>
       </c>
       <c r="F48" t="n">
-        <v>136.2951965332031</v>
+        <v>136.6499938964844</v>
       </c>
       <c r="G48" t="n">
-        <v>2725.903930664062</v>
+        <v>2732.999877929688</v>
       </c>
       <c r="H48" t="n">
-        <v>0.1536798134149128</v>
+        <v>0.1540182502711204</v>
       </c>
     </row>
     <row r="49">
@@ -1911,7 +1911,7 @@
         <v>3017.999877929688</v>
       </c>
       <c r="H49" t="n">
-        <v>0.1606830912658308</v>
+        <v>0.1605961443530085</v>
       </c>
     </row>
     <row r="50">
@@ -1941,7 +1941,7 @@
         <v>10710.68027496338</v>
       </c>
       <c r="H50" t="n">
-        <v>0.5702535738078549</v>
+        <v>0.5699450050133548</v>
       </c>
     </row>
     <row r="51">
@@ -1971,7 +1971,7 @@
         <v>1147.300048828125</v>
       </c>
       <c r="H51" t="n">
-        <v>0.06108407087862602</v>
+        <v>0.06105101779666405</v>
       </c>
     </row>
     <row r="52">
@@ -1995,13 +1995,13 @@
         </is>
       </c>
       <c r="F52" t="n">
-        <v>130.2110443115234</v>
+        <v>130.5500030517578</v>
       </c>
       <c r="G52" t="n">
-        <v>3906.331329345703</v>
+        <v>3916.500091552734</v>
       </c>
       <c r="H52" t="n">
-        <v>0.2079792640476884</v>
+        <v>0.2084078328369726</v>
       </c>
     </row>
     <row r="53">
@@ -2031,7 +2031,7 @@
         <v>1831.999969482422</v>
       </c>
       <c r="H53" t="n">
-        <v>0.1182621707680098</v>
+        <v>0.1182164291121852</v>
       </c>
     </row>
     <row r="54">
@@ -2061,7 +2061,7 @@
         <v>10534.99984741211</v>
       </c>
       <c r="H54" t="n">
-        <v>0.6800720369813099</v>
+        <v>0.6798089974915936</v>
       </c>
     </row>
     <row r="55">
@@ -2091,7 +2091,7 @@
         <v>821.5</v>
       </c>
       <c r="H55" t="n">
-        <v>0.05303077232766965</v>
+        <v>0.05301026098984984</v>
       </c>
     </row>
     <row r="56">
@@ -2115,13 +2115,13 @@
         </is>
       </c>
       <c r="F56" t="n">
-        <v>76.75019836425781</v>
+        <v>76.94999694824219</v>
       </c>
       <c r="G56" t="n">
-        <v>2302.505950927734</v>
+        <v>2308.499908447266</v>
       </c>
       <c r="H56" t="n">
-        <v>0.1486350199230106</v>
+        <v>0.1489643124063713</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Reworked computation of de_adjusting closing price to [fix #7]
This is the second and final step of the bugfix.

The adjusted_price is not passed to the de_adjustment function any more.
Instead the de_adjustment function simply returns the de_adjustment factor
(if exists), then the caller does the computation.
</commit_message>
<xml_diff>
--- a/multibeggar/tests/output/test_transactions_list_small_daywise_full_portfolio.xlsx
+++ b/multibeggar/tests/output/test_transactions_list_small_daywise_full_portfolio.xlsx
@@ -521,7 +521,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>[None, 'BLACKROSE.BO']</t>
+          <t>['BLACKROSE.BO']</t>
         </is>
       </c>
       <c r="F3" t="n">
@@ -581,7 +581,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>[None, 'BLACKROSE.BO']</t>
+          <t>['BLACKROSE.BO']</t>
         </is>
       </c>
       <c r="F5" t="n">
@@ -641,7 +641,7 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>[None, 'BLACKROSE.BO']</t>
+          <t>['BLACKROSE.BO']</t>
         </is>
       </c>
       <c r="F7" t="n">
@@ -701,7 +701,7 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>[None, 'BLACKROSE.BO']</t>
+          <t>['BLACKROSE.BO']</t>
         </is>
       </c>
       <c r="F9" t="n">
@@ -761,7 +761,7 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>[None, 'BLACKROSE.BO']</t>
+          <t>['BLACKROSE.BO']</t>
         </is>
       </c>
       <c r="F11" t="n">
@@ -851,7 +851,7 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>[None, 'BLACKROSE.BO']</t>
+          <t>['BLACKROSE.BO']</t>
         </is>
       </c>
       <c r="F14" t="n">
@@ -911,7 +911,7 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>[None, 'BLACKROSE.BO']</t>
+          <t>['BLACKROSE.BO']</t>
         </is>
       </c>
       <c r="F16" t="n">
@@ -1001,7 +1001,7 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>[None, 'BLACKROSE.BO']</t>
+          <t>['BLACKROSE.BO']</t>
         </is>
       </c>
       <c r="F19" t="n">
@@ -1121,7 +1121,7 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>[None, 'BLACKROSE.BO']</t>
+          <t>['BLACKROSE.BO']</t>
         </is>
       </c>
       <c r="F23" t="n">
@@ -1241,7 +1241,7 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>[None, 'BLACKROSE.BO']</t>
+          <t>['BLACKROSE.BO']</t>
         </is>
       </c>
       <c r="F27" t="n">
@@ -1361,7 +1361,7 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>[None, 'BLACKROSE.BO']</t>
+          <t>['BLACKROSE.BO']</t>
         </is>
       </c>
       <c r="F31" t="n">
@@ -1631,7 +1631,7 @@
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>[None, 'BLACKROSE.BO']</t>
+          <t>['BLACKROSE.BO']</t>
         </is>
       </c>
       <c r="F40" t="n">
@@ -1751,7 +1751,7 @@
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>[None, 'BLACKROSE.BO']</t>
+          <t>['BLACKROSE.BO']</t>
         </is>
       </c>
       <c r="F44" t="n">
@@ -1871,7 +1871,7 @@
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>[None, 'BLACKROSE.BO']</t>
+          <t>['BLACKROSE.BO']</t>
         </is>
       </c>
       <c r="F48" t="n">
@@ -1991,7 +1991,7 @@
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>[None, 'BLACKROSE.BO']</t>
+          <t>['BLACKROSE.BO']</t>
         </is>
       </c>
       <c r="F52" t="n">
@@ -2111,7 +2111,7 @@
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>[None, 'BLACKROSE.BO']</t>
+          <t>['BLACKROSE.BO']</t>
         </is>
       </c>
       <c r="F56" t="n">

</xml_diff>

<commit_message>
Reworked computation of de_adjusting closing price to fix#7
This is the second and final step of the bugfix.

The adjusted_price is not passed to the de_adjustment function any more.
Instead the de_adjustment function simply returns the de_adjustment factor
(if exists), then the caller does the computation.
</commit_message>
<xml_diff>
--- a/multibeggar/tests/output/test_transactions_list_small_daywise_full_portfolio.xlsx
+++ b/multibeggar/tests/output/test_transactions_list_small_daywise_full_portfolio.xlsx
@@ -521,7 +521,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>[None, 'BLACKROSE.BO']</t>
+          <t>['BLACKROSE.BO']</t>
         </is>
       </c>
       <c r="F3" t="n">
@@ -581,7 +581,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>[None, 'BLACKROSE.BO']</t>
+          <t>['BLACKROSE.BO']</t>
         </is>
       </c>
       <c r="F5" t="n">
@@ -641,7 +641,7 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>[None, 'BLACKROSE.BO']</t>
+          <t>['BLACKROSE.BO']</t>
         </is>
       </c>
       <c r="F7" t="n">
@@ -701,7 +701,7 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>[None, 'BLACKROSE.BO']</t>
+          <t>['BLACKROSE.BO']</t>
         </is>
       </c>
       <c r="F9" t="n">
@@ -761,7 +761,7 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>[None, 'BLACKROSE.BO']</t>
+          <t>['BLACKROSE.BO']</t>
         </is>
       </c>
       <c r="F11" t="n">
@@ -851,7 +851,7 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>[None, 'BLACKROSE.BO']</t>
+          <t>['BLACKROSE.BO']</t>
         </is>
       </c>
       <c r="F14" t="n">
@@ -911,7 +911,7 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>[None, 'BLACKROSE.BO']</t>
+          <t>['BLACKROSE.BO']</t>
         </is>
       </c>
       <c r="F16" t="n">
@@ -1001,7 +1001,7 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>[None, 'BLACKROSE.BO']</t>
+          <t>['BLACKROSE.BO']</t>
         </is>
       </c>
       <c r="F19" t="n">
@@ -1121,7 +1121,7 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>[None, 'BLACKROSE.BO']</t>
+          <t>['BLACKROSE.BO']</t>
         </is>
       </c>
       <c r="F23" t="n">
@@ -1241,7 +1241,7 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>[None, 'BLACKROSE.BO']</t>
+          <t>['BLACKROSE.BO']</t>
         </is>
       </c>
       <c r="F27" t="n">
@@ -1361,7 +1361,7 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>[None, 'BLACKROSE.BO']</t>
+          <t>['BLACKROSE.BO']</t>
         </is>
       </c>
       <c r="F31" t="n">
@@ -1631,7 +1631,7 @@
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>[None, 'BLACKROSE.BO']</t>
+          <t>['BLACKROSE.BO']</t>
         </is>
       </c>
       <c r="F40" t="n">
@@ -1751,7 +1751,7 @@
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>[None, 'BLACKROSE.BO']</t>
+          <t>['BLACKROSE.BO']</t>
         </is>
       </c>
       <c r="F44" t="n">
@@ -1871,7 +1871,7 @@
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>[None, 'BLACKROSE.BO']</t>
+          <t>['BLACKROSE.BO']</t>
         </is>
       </c>
       <c r="F48" t="n">
@@ -1991,7 +1991,7 @@
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>[None, 'BLACKROSE.BO']</t>
+          <t>['BLACKROSE.BO']</t>
         </is>
       </c>
       <c r="F52" t="n">
@@ -2111,7 +2111,7 @@
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>[None, 'BLACKROSE.BO']</t>
+          <t>['BLACKROSE.BO']</t>
         </is>
       </c>
       <c r="F56" t="n">

</xml_diff>

<commit_message>
Ignore holdings with invalid closing_price to compute complexity [fix #12]
</commit_message>
<xml_diff>
--- a/multibeggar/tests/output/test_transactions_list_small_daywise_full_portfolio.xlsx
+++ b/multibeggar/tests/output/test_transactions_list_small_daywise_full_portfolio.xlsx
@@ -561,7 +561,7 @@
         <v>487.3875045776367</v>
       </c>
       <c r="H4" t="n">
-        <v>0.2320683912910165</v>
+        <v>0.2316053946019448</v>
       </c>
     </row>
     <row r="5">
@@ -585,13 +585,13 @@
         </is>
       </c>
       <c r="F5" t="n">
-        <v>80.64007949829102</v>
+        <v>80.85000133514404</v>
       </c>
       <c r="G5" t="n">
-        <v>1612.80158996582</v>
+        <v>1617.000026702881</v>
       </c>
       <c r="H5" t="n">
-        <v>0.7679316087089835</v>
+        <v>0.7683946053980552</v>
       </c>
     </row>
     <row r="6">
@@ -891,7 +891,7 @@
         <v>1990</v>
       </c>
       <c r="H15" t="n">
-        <v>0.1897198552766218</v>
+        <v>0.2684654355432816</v>
       </c>
     </row>
     <row r="16">
@@ -921,7 +921,7 @@
         <v>5422.499847412109</v>
       </c>
       <c r="H16" t="n">
-        <v>0.516962756928909</v>
+        <v>0.7315345644567185</v>
       </c>
     </row>
     <row r="17">
@@ -944,15 +944,9 @@
           <t>['MON100.NS', 'MON100.BO']</t>
         </is>
       </c>
-      <c r="F17" t="n">
-        <v>615.3300094604492</v>
-      </c>
-      <c r="G17" t="n">
-        <v>3076.650047302246</v>
-      </c>
-      <c r="H17" t="n">
-        <v>0.2933173877944692</v>
-      </c>
+      <c r="F17" t="inlineStr"/>
+      <c r="G17" t="inlineStr"/>
+      <c r="H17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
@@ -981,7 +975,7 @@
         <v>2529.999923706055</v>
       </c>
       <c r="H18" t="n">
-        <v>0.1963294899032366</v>
+        <v>0.258063197744421</v>
       </c>
     </row>
     <row r="19">
@@ -1011,7 +1005,7 @@
         <v>6071.999816894531</v>
       </c>
       <c r="H19" t="n">
-        <v>0.471190775767768</v>
+        <v>0.6193516745866104</v>
       </c>
     </row>
     <row r="20">
@@ -1034,15 +1028,9 @@
           <t>['MON100.NS', 'MON100.BO']</t>
         </is>
       </c>
-      <c r="F20" t="n">
-        <v>616.5399932861328</v>
-      </c>
-      <c r="G20" t="n">
-        <v>3082.699966430664</v>
-      </c>
-      <c r="H20" t="n">
-        <v>0.2392193399940886</v>
-      </c>
+      <c r="F20" t="inlineStr"/>
+      <c r="G20" t="inlineStr"/>
+      <c r="H20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
@@ -1071,7 +1059,7 @@
         <v>1201.800048828125</v>
       </c>
       <c r="H21" t="n">
-        <v>0.09326039433490677</v>
+        <v>0.1225851276689685</v>
       </c>
     </row>
     <row r="22">
@@ -1101,7 +1089,7 @@
         <v>3325.499954223633</v>
       </c>
       <c r="H22" t="n">
-        <v>0.2342788964336497</v>
+        <v>0.3189744396683761</v>
       </c>
     </row>
     <row r="23">
@@ -1131,7 +1119,7 @@
         <v>5853.000183105469</v>
       </c>
       <c r="H23" t="n">
-        <v>0.4123393302057723</v>
+        <v>0.561406549235941</v>
       </c>
     </row>
     <row r="24">
@@ -1154,15 +1142,9 @@
           <t>['MON100.NS', 'MON100.BO']</t>
         </is>
       </c>
-      <c r="F24" t="n">
-        <v>628.1700134277344</v>
-      </c>
-      <c r="G24" t="n">
-        <v>3769.020080566406</v>
-      </c>
-      <c r="H24" t="n">
-        <v>0.2655245458626109</v>
-      </c>
+      <c r="F24" t="inlineStr"/>
+      <c r="G24" t="inlineStr"/>
+      <c r="H24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" s="1" t="n">
@@ -1191,7 +1173,7 @@
         <v>1247.099975585938</v>
       </c>
       <c r="H25" t="n">
-        <v>0.08785722749796712</v>
+        <v>0.119619011095683</v>
       </c>
     </row>
     <row r="26">
@@ -1221,7 +1203,7 @@
         <v>3185.999908447266</v>
       </c>
       <c r="H26" t="n">
-        <v>0.2200738230840038</v>
+        <v>0.3190274972322454</v>
       </c>
     </row>
     <row r="27">
@@ -1251,7 +1233,7 @@
         <v>5546.999816894531</v>
       </c>
       <c r="H27" t="n">
-        <v>0.3831605434493547</v>
+        <v>0.5554442936547488</v>
       </c>
     </row>
     <row r="28">
@@ -1274,15 +1256,9 @@
           <t>['MON100.NS', 'MON100.BO']</t>
         </is>
       </c>
-      <c r="F28" t="n">
-        <v>641.4800262451172</v>
-      </c>
-      <c r="G28" t="n">
-        <v>4490.36018371582</v>
-      </c>
-      <c r="H28" t="n">
-        <v>0.3101728691311063</v>
-      </c>
+      <c r="F28" t="inlineStr"/>
+      <c r="G28" t="inlineStr"/>
+      <c r="H28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" s="1" t="n">
@@ -1311,7 +1287,7 @@
         <v>1253.599975585938</v>
       </c>
       <c r="H29" t="n">
-        <v>0.0865927643355353</v>
+        <v>0.1255282091130058</v>
       </c>
     </row>
     <row r="30">
@@ -1341,7 +1317,7 @@
         <v>3596.25</v>
       </c>
       <c r="H30" t="n">
-        <v>0.2105908844293644</v>
+        <v>0.335992937557209</v>
       </c>
     </row>
     <row r="31">
@@ -1371,7 +1347,7 @@
         <v>5865</v>
       </c>
       <c r="H31" t="n">
-        <v>0.343445404846221</v>
+        <v>0.5479592850255212</v>
       </c>
     </row>
     <row r="32">
@@ -1394,15 +1370,9 @@
           <t>['MON100.NS', 'MON100.BO']</t>
         </is>
       </c>
-      <c r="F32" t="n">
-        <v>637.3600006103516</v>
-      </c>
-      <c r="G32" t="n">
-        <v>6373.600006103516</v>
-      </c>
-      <c r="H32" t="n">
-        <v>0.3732282411635292</v>
-      </c>
+      <c r="F32" t="inlineStr"/>
+      <c r="G32" t="inlineStr"/>
+      <c r="H32" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" s="1" t="n">
@@ -1431,7 +1401,7 @@
         <v>1242.099975585938</v>
       </c>
       <c r="H33" t="n">
-        <v>0.0727354695608855</v>
+        <v>0.1160477774172698</v>
       </c>
     </row>
     <row r="34">
@@ -1461,7 +1431,7 @@
         <v>3437.175037384033</v>
       </c>
       <c r="H34" t="n">
-        <v>0.3066465430776691</v>
+        <v>0.7288010183144951</v>
       </c>
     </row>
     <row r="35">
@@ -1484,15 +1454,9 @@
           <t>['MON100.NS', 'MON100.BO']</t>
         </is>
       </c>
-      <c r="F35" t="n">
-        <v>649.27099609375</v>
-      </c>
-      <c r="G35" t="n">
-        <v>6492.7099609375</v>
-      </c>
-      <c r="H35" t="n">
-        <v>0.5792451775289043</v>
-      </c>
+      <c r="F35" t="inlineStr"/>
+      <c r="G35" t="inlineStr"/>
+      <c r="H35" t="inlineStr"/>
     </row>
     <row r="36">
       <c r="A36" s="1" t="n">
@@ -1521,7 +1485,7 @@
         <v>1279.030004882813</v>
       </c>
       <c r="H36" t="n">
-        <v>0.1141082793934266</v>
+        <v>0.271198981685505</v>
       </c>
     </row>
     <row r="37">
@@ -1551,7 +1515,7 @@
         <v>3318.000106811523</v>
       </c>
       <c r="H37" t="n">
-        <v>0.2756603970605329</v>
+        <v>0.6177908171852359</v>
       </c>
     </row>
     <row r="38">
@@ -1574,15 +1538,9 @@
           <t>['MON100.NS', 'MON100.BO']</t>
         </is>
       </c>
-      <c r="F38" t="n">
-        <v>666.5799713134766</v>
-      </c>
-      <c r="G38" t="n">
-        <v>6665.799713134766</v>
-      </c>
-      <c r="H38" t="n">
-        <v>0.5537965450563179</v>
-      </c>
+      <c r="F38" t="inlineStr"/>
+      <c r="G38" t="inlineStr"/>
+      <c r="H38" t="inlineStr"/>
     </row>
     <row r="39">
       <c r="A39" s="1" t="n">
@@ -1611,7 +1569,7 @@
         <v>1365</v>
       </c>
       <c r="H39" t="n">
-        <v>0.1134045900767662</v>
+        <v>0.2541544419262278</v>
       </c>
     </row>
     <row r="40">
@@ -1641,7 +1599,7 @@
         <v>687.7500152587891</v>
       </c>
       <c r="H40" t="n">
-        <v>0.05713846780638292</v>
+        <v>0.1280547408885364</v>
       </c>
     </row>
     <row r="41">
@@ -1671,7 +1629,7 @@
         <v>3722.000122070312</v>
       </c>
       <c r="H41" t="n">
-        <v>0.2675888384137958</v>
+        <v>0.5110882398178012</v>
       </c>
     </row>
     <row r="42">
@@ -1694,15 +1652,9 @@
           <t>['MON100.NS', 'MON100.BO']</t>
         </is>
       </c>
-      <c r="F42" t="n">
-        <v>662.6899719238281</v>
-      </c>
-      <c r="G42" t="n">
-        <v>6626.899719238281</v>
-      </c>
-      <c r="H42" t="n">
-        <v>0.4764331918316316</v>
-      </c>
+      <c r="F42" t="inlineStr"/>
+      <c r="G42" t="inlineStr"/>
+      <c r="H42" t="inlineStr"/>
     </row>
     <row r="43">
       <c r="A43" s="1" t="n">
@@ -1731,7 +1683,7 @@
         <v>1327</v>
       </c>
       <c r="H43" t="n">
-        <v>0.09540311040548617</v>
+        <v>0.1822176442758886</v>
       </c>
     </row>
     <row r="44">
@@ -1761,7 +1713,7 @@
         <v>2233.499908447266</v>
       </c>
       <c r="H44" t="n">
-        <v>0.1605748593490865</v>
+        <v>0.3066941159063102</v>
       </c>
     </row>
     <row r="45">
@@ -1791,7 +1743,7 @@
         <v>3473.999938964844</v>
       </c>
       <c r="H45" t="n">
-        <v>0.1957773201390204</v>
+        <v>0.4631752989796255</v>
       </c>
     </row>
     <row r="46">
@@ -1814,15 +1766,9 @@
           <t>['MON100.NS', 'MON100.BO']</t>
         </is>
       </c>
-      <c r="F46" t="n">
-        <v>682.9499816894531</v>
-      </c>
-      <c r="G46" t="n">
-        <v>10244.2497253418</v>
-      </c>
-      <c r="H46" t="n">
-        <v>0.5773148512662105</v>
-      </c>
+      <c r="F46" t="inlineStr"/>
+      <c r="G46" t="inlineStr"/>
+      <c r="H46" t="inlineStr"/>
     </row>
     <row r="47">
       <c r="A47" s="1" t="n">
@@ -1851,7 +1797,7 @@
         <v>1293.400024414062</v>
       </c>
       <c r="H47" t="n">
-        <v>0.07288957832364869</v>
+        <v>0.1724441432162906</v>
       </c>
     </row>
     <row r="48">
@@ -1881,7 +1827,7 @@
         <v>2732.999877929688</v>
       </c>
       <c r="H48" t="n">
-        <v>0.1540182502711204</v>
+        <v>0.3643805578040838</v>
       </c>
     </row>
     <row r="49">
@@ -1911,7 +1857,7 @@
         <v>3017.999877929688</v>
       </c>
       <c r="H49" t="n">
-        <v>0.1605961443530085</v>
+        <v>0.3734316453131666</v>
       </c>
     </row>
     <row r="50">
@@ -1934,15 +1880,9 @@
           <t>['MON100.NS', 'MON100.BO']</t>
         </is>
       </c>
-      <c r="F50" t="n">
-        <v>630.0400161743164</v>
-      </c>
-      <c r="G50" t="n">
-        <v>10710.68027496338</v>
-      </c>
-      <c r="H50" t="n">
-        <v>0.5699450050133548</v>
-      </c>
+      <c r="F50" t="inlineStr"/>
+      <c r="G50" t="inlineStr"/>
+      <c r="H50" t="inlineStr"/>
     </row>
     <row r="51">
       <c r="A51" s="1" t="n">
@@ -1971,7 +1911,7 @@
         <v>1147.300048828125</v>
       </c>
       <c r="H51" t="n">
-        <v>0.06105101779666405</v>
+        <v>0.1419609550135789</v>
       </c>
     </row>
     <row r="52">
@@ -2001,7 +1941,7 @@
         <v>3916.500091552734</v>
       </c>
       <c r="H52" t="n">
-        <v>0.2084078328369726</v>
+        <v>0.4846073996732544</v>
       </c>
     </row>
     <row r="53">
@@ -2031,7 +1971,7 @@
         <v>1831.999969482422</v>
       </c>
       <c r="H53" t="n">
-        <v>0.1182164291121852</v>
+        <v>0.3692059682691475</v>
       </c>
     </row>
     <row r="54">
@@ -2054,15 +1994,9 @@
           <t>['MON100.NS', 'MON100.BO']</t>
         </is>
       </c>
-      <c r="F54" t="n">
-        <v>526.7499923706055</v>
-      </c>
-      <c r="G54" t="n">
-        <v>10534.99984741211</v>
-      </c>
-      <c r="H54" t="n">
-        <v>0.6798089974915936</v>
-      </c>
+      <c r="F54" t="inlineStr"/>
+      <c r="G54" t="inlineStr"/>
+      <c r="H54" t="inlineStr"/>
     </row>
     <row r="55">
       <c r="A55" s="1" t="n">
@@ -2091,7 +2025,7 @@
         <v>821.5</v>
       </c>
       <c r="H55" t="n">
-        <v>0.05301026098984984</v>
+        <v>0.1655582467169986</v>
       </c>
     </row>
     <row r="56">
@@ -2121,7 +2055,7 @@
         <v>2308.499908447266</v>
       </c>
       <c r="H56" t="n">
-        <v>0.1489643124063713</v>
+        <v>0.4652357850138539</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Cleaned up obsolete code that fetched stock data from server if not found in prefetched data [close #17]
This is the third and final step of the refactoring for #17.
</commit_message>
<xml_diff>
--- a/multibeggar/tests/output/test_transactions_list_small_daywise_full_portfolio.xlsx
+++ b/multibeggar/tests/output/test_transactions_list_small_daywise_full_portfolio.xlsx
@@ -891,7 +891,7 @@
         <v>1990</v>
       </c>
       <c r="H15" t="n">
-        <v>0.2684654355432816</v>
+        <v>0.1897198552766218</v>
       </c>
     </row>
     <row r="16">
@@ -921,7 +921,7 @@
         <v>5422.499847412109</v>
       </c>
       <c r="H16" t="n">
-        <v>0.7315345644567185</v>
+        <v>0.516962756928909</v>
       </c>
     </row>
     <row r="17">
@@ -944,9 +944,15 @@
           <t>['MON100.NS', 'MON100.BO']</t>
         </is>
       </c>
-      <c r="F17" t="inlineStr"/>
-      <c r="G17" t="inlineStr"/>
-      <c r="H17" t="inlineStr"/>
+      <c r="F17" t="n">
+        <v>615.3300094604492</v>
+      </c>
+      <c r="G17" t="n">
+        <v>3076.650047302246</v>
+      </c>
+      <c r="H17" t="n">
+        <v>0.2933173877944692</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
@@ -975,7 +981,7 @@
         <v>2529.999923706055</v>
       </c>
       <c r="H18" t="n">
-        <v>0.258063197744421</v>
+        <v>0.1963294899032366</v>
       </c>
     </row>
     <row r="19">
@@ -1005,7 +1011,7 @@
         <v>6071.999816894531</v>
       </c>
       <c r="H19" t="n">
-        <v>0.6193516745866104</v>
+        <v>0.471190775767768</v>
       </c>
     </row>
     <row r="20">
@@ -1028,9 +1034,15 @@
           <t>['MON100.NS', 'MON100.BO']</t>
         </is>
       </c>
-      <c r="F20" t="inlineStr"/>
-      <c r="G20" t="inlineStr"/>
-      <c r="H20" t="inlineStr"/>
+      <c r="F20" t="n">
+        <v>616.5399932861328</v>
+      </c>
+      <c r="G20" t="n">
+        <v>3082.699966430664</v>
+      </c>
+      <c r="H20" t="n">
+        <v>0.2392193399940886</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
@@ -1059,7 +1071,7 @@
         <v>1201.800048828125</v>
       </c>
       <c r="H21" t="n">
-        <v>0.1225851276689685</v>
+        <v>0.09326039433490677</v>
       </c>
     </row>
     <row r="22">
@@ -1089,7 +1101,7 @@
         <v>3325.499954223633</v>
       </c>
       <c r="H22" t="n">
-        <v>0.3189744396683761</v>
+        <v>0.2342788964336497</v>
       </c>
     </row>
     <row r="23">
@@ -1119,7 +1131,7 @@
         <v>5853.000183105469</v>
       </c>
       <c r="H23" t="n">
-        <v>0.561406549235941</v>
+        <v>0.4123393302057723</v>
       </c>
     </row>
     <row r="24">
@@ -1142,9 +1154,15 @@
           <t>['MON100.NS', 'MON100.BO']</t>
         </is>
       </c>
-      <c r="F24" t="inlineStr"/>
-      <c r="G24" t="inlineStr"/>
-      <c r="H24" t="inlineStr"/>
+      <c r="F24" t="n">
+        <v>628.1700134277344</v>
+      </c>
+      <c r="G24" t="n">
+        <v>3769.020080566406</v>
+      </c>
+      <c r="H24" t="n">
+        <v>0.2655245458626109</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="n">
@@ -1173,7 +1191,7 @@
         <v>1247.099975585938</v>
       </c>
       <c r="H25" t="n">
-        <v>0.119619011095683</v>
+        <v>0.08785722749796712</v>
       </c>
     </row>
     <row r="26">
@@ -1203,7 +1221,7 @@
         <v>3185.999908447266</v>
       </c>
       <c r="H26" t="n">
-        <v>0.3190274972322454</v>
+        <v>0.2200738230840038</v>
       </c>
     </row>
     <row r="27">
@@ -1233,7 +1251,7 @@
         <v>5546.999816894531</v>
       </c>
       <c r="H27" t="n">
-        <v>0.5554442936547488</v>
+        <v>0.3831605434493547</v>
       </c>
     </row>
     <row r="28">
@@ -1256,9 +1274,15 @@
           <t>['MON100.NS', 'MON100.BO']</t>
         </is>
       </c>
-      <c r="F28" t="inlineStr"/>
-      <c r="G28" t="inlineStr"/>
-      <c r="H28" t="inlineStr"/>
+      <c r="F28" t="n">
+        <v>641.4800262451172</v>
+      </c>
+      <c r="G28" t="n">
+        <v>4490.36018371582</v>
+      </c>
+      <c r="H28" t="n">
+        <v>0.3101728691311063</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="n">
@@ -1287,7 +1311,7 @@
         <v>1253.599975585938</v>
       </c>
       <c r="H29" t="n">
-        <v>0.1255282091130058</v>
+        <v>0.0865927643355353</v>
       </c>
     </row>
     <row r="30">
@@ -1317,7 +1341,7 @@
         <v>3596.25</v>
       </c>
       <c r="H30" t="n">
-        <v>0.335992937557209</v>
+        <v>0.2105908844293644</v>
       </c>
     </row>
     <row r="31">
@@ -1347,7 +1371,7 @@
         <v>5865</v>
       </c>
       <c r="H31" t="n">
-        <v>0.5479592850255212</v>
+        <v>0.343445404846221</v>
       </c>
     </row>
     <row r="32">
@@ -1370,9 +1394,15 @@
           <t>['MON100.NS', 'MON100.BO']</t>
         </is>
       </c>
-      <c r="F32" t="inlineStr"/>
-      <c r="G32" t="inlineStr"/>
-      <c r="H32" t="inlineStr"/>
+      <c r="F32" t="n">
+        <v>637.3600006103516</v>
+      </c>
+      <c r="G32" t="n">
+        <v>6373.600006103516</v>
+      </c>
+      <c r="H32" t="n">
+        <v>0.3732282411635292</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="n">
@@ -1401,7 +1431,7 @@
         <v>1242.099975585938</v>
       </c>
       <c r="H33" t="n">
-        <v>0.1160477774172698</v>
+        <v>0.0727354695608855</v>
       </c>
     </row>
     <row r="34">
@@ -1431,7 +1461,7 @@
         <v>3437.175037384033</v>
       </c>
       <c r="H34" t="n">
-        <v>0.7288010183144951</v>
+        <v>0.3066465430776691</v>
       </c>
     </row>
     <row r="35">
@@ -1454,9 +1484,15 @@
           <t>['MON100.NS', 'MON100.BO']</t>
         </is>
       </c>
-      <c r="F35" t="inlineStr"/>
-      <c r="G35" t="inlineStr"/>
-      <c r="H35" t="inlineStr"/>
+      <c r="F35" t="n">
+        <v>649.27099609375</v>
+      </c>
+      <c r="G35" t="n">
+        <v>6492.7099609375</v>
+      </c>
+      <c r="H35" t="n">
+        <v>0.5792451775289043</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="n">
@@ -1485,7 +1521,7 @@
         <v>1279.030004882813</v>
       </c>
       <c r="H36" t="n">
-        <v>0.271198981685505</v>
+        <v>0.1141082793934266</v>
       </c>
     </row>
     <row r="37">
@@ -1515,7 +1551,7 @@
         <v>3318.000106811523</v>
       </c>
       <c r="H37" t="n">
-        <v>0.6177908171852359</v>
+        <v>0.2756603970605329</v>
       </c>
     </row>
     <row r="38">
@@ -1538,9 +1574,15 @@
           <t>['MON100.NS', 'MON100.BO']</t>
         </is>
       </c>
-      <c r="F38" t="inlineStr"/>
-      <c r="G38" t="inlineStr"/>
-      <c r="H38" t="inlineStr"/>
+      <c r="F38" t="n">
+        <v>666.5799713134766</v>
+      </c>
+      <c r="G38" t="n">
+        <v>6665.799713134766</v>
+      </c>
+      <c r="H38" t="n">
+        <v>0.5537965450563179</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="n">
@@ -1569,7 +1611,7 @@
         <v>1365</v>
       </c>
       <c r="H39" t="n">
-        <v>0.2541544419262278</v>
+        <v>0.1134045900767662</v>
       </c>
     </row>
     <row r="40">
@@ -1599,7 +1641,7 @@
         <v>687.7500152587891</v>
       </c>
       <c r="H40" t="n">
-        <v>0.1280547408885364</v>
+        <v>0.05713846780638292</v>
       </c>
     </row>
     <row r="41">
@@ -1629,7 +1671,7 @@
         <v>3722.000122070312</v>
       </c>
       <c r="H41" t="n">
-        <v>0.5110882398178012</v>
+        <v>0.2675888384137958</v>
       </c>
     </row>
     <row r="42">
@@ -1652,9 +1694,15 @@
           <t>['MON100.NS', 'MON100.BO']</t>
         </is>
       </c>
-      <c r="F42" t="inlineStr"/>
-      <c r="G42" t="inlineStr"/>
-      <c r="H42" t="inlineStr"/>
+      <c r="F42" t="n">
+        <v>662.6899719238281</v>
+      </c>
+      <c r="G42" t="n">
+        <v>6626.899719238281</v>
+      </c>
+      <c r="H42" t="n">
+        <v>0.4764331918316316</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="n">
@@ -1683,7 +1731,7 @@
         <v>1327</v>
       </c>
       <c r="H43" t="n">
-        <v>0.1822176442758886</v>
+        <v>0.09540311040548617</v>
       </c>
     </row>
     <row r="44">
@@ -1713,7 +1761,7 @@
         <v>2233.499908447266</v>
       </c>
       <c r="H44" t="n">
-        <v>0.3066941159063102</v>
+        <v>0.1605748593490865</v>
       </c>
     </row>
     <row r="45">
@@ -1743,7 +1791,7 @@
         <v>3473.999938964844</v>
       </c>
       <c r="H45" t="n">
-        <v>0.4631752989796255</v>
+        <v>0.1957773201390204</v>
       </c>
     </row>
     <row r="46">
@@ -1766,9 +1814,15 @@
           <t>['MON100.NS', 'MON100.BO']</t>
         </is>
       </c>
-      <c r="F46" t="inlineStr"/>
-      <c r="G46" t="inlineStr"/>
-      <c r="H46" t="inlineStr"/>
+      <c r="F46" t="n">
+        <v>682.9499816894531</v>
+      </c>
+      <c r="G46" t="n">
+        <v>10244.2497253418</v>
+      </c>
+      <c r="H46" t="n">
+        <v>0.5773148512662105</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47" s="1" t="n">
@@ -1797,7 +1851,7 @@
         <v>1293.400024414062</v>
       </c>
       <c r="H47" t="n">
-        <v>0.1724441432162906</v>
+        <v>0.07288957832364869</v>
       </c>
     </row>
     <row r="48">
@@ -1827,7 +1881,7 @@
         <v>2732.999877929688</v>
       </c>
       <c r="H48" t="n">
-        <v>0.3643805578040838</v>
+        <v>0.1540182502711204</v>
       </c>
     </row>
     <row r="49">
@@ -1857,7 +1911,7 @@
         <v>3017.999877929688</v>
       </c>
       <c r="H49" t="n">
-        <v>0.3734316453131666</v>
+        <v>0.1605961443530085</v>
       </c>
     </row>
     <row r="50">
@@ -1880,9 +1934,15 @@
           <t>['MON100.NS', 'MON100.BO']</t>
         </is>
       </c>
-      <c r="F50" t="inlineStr"/>
-      <c r="G50" t="inlineStr"/>
-      <c r="H50" t="inlineStr"/>
+      <c r="F50" t="n">
+        <v>630.0400161743164</v>
+      </c>
+      <c r="G50" t="n">
+        <v>10710.68027496338</v>
+      </c>
+      <c r="H50" t="n">
+        <v>0.5699450050133548</v>
+      </c>
     </row>
     <row r="51">
       <c r="A51" s="1" t="n">
@@ -1911,7 +1971,7 @@
         <v>1147.300048828125</v>
       </c>
       <c r="H51" t="n">
-        <v>0.1419609550135789</v>
+        <v>0.06105101779666405</v>
       </c>
     </row>
     <row r="52">
@@ -1941,7 +2001,7 @@
         <v>3916.500091552734</v>
       </c>
       <c r="H52" t="n">
-        <v>0.4846073996732544</v>
+        <v>0.2084078328369726</v>
       </c>
     </row>
     <row r="53">
@@ -1971,7 +2031,7 @@
         <v>1831.999969482422</v>
       </c>
       <c r="H53" t="n">
-        <v>0.3692059682691475</v>
+        <v>0.1182164291121852</v>
       </c>
     </row>
     <row r="54">
@@ -1994,9 +2054,15 @@
           <t>['MON100.NS', 'MON100.BO']</t>
         </is>
       </c>
-      <c r="F54" t="inlineStr"/>
-      <c r="G54" t="inlineStr"/>
-      <c r="H54" t="inlineStr"/>
+      <c r="F54" t="n">
+        <v>526.7499923706055</v>
+      </c>
+      <c r="G54" t="n">
+        <v>10534.99984741211</v>
+      </c>
+      <c r="H54" t="n">
+        <v>0.6798089974915936</v>
+      </c>
     </row>
     <row r="55">
       <c r="A55" s="1" t="n">
@@ -2025,7 +2091,7 @@
         <v>821.5</v>
       </c>
       <c r="H55" t="n">
-        <v>0.1655582467169986</v>
+        <v>0.05301026098984984</v>
       </c>
     </row>
     <row r="56">
@@ -2055,7 +2121,7 @@
         <v>2308.499908447266</v>
       </c>
       <c r="H56" t="n">
-        <v>0.4652357850138539</v>
+        <v>0.1489643124063713</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
pushing all the updated files
</commit_message>
<xml_diff>
--- a/multibeggar/tests/output/test_transactions_list_small_daywise_full_portfolio.xlsx
+++ b/multibeggar/tests/output/test_transactions_list_small_daywise_full_portfolio.xlsx
@@ -491,7 +491,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>['ABCAPITAL.NS', 'ABCAPITAL.BO']</t>
+          <t>[('ABCAPITAL', &lt;StockExchange.NSE: 'NSE'&gt;), ('ABCAPITAL', &lt;StockExchange.BSE: 'BSE'&gt;)]</t>
         </is>
       </c>
       <c r="F2" t="n">
@@ -521,7 +521,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>['BLACKROSE.BO']</t>
+          <t>[('BLACKROSE', &lt;StockExchange.BSE: 'BSE'&gt;)]</t>
         </is>
       </c>
       <c r="F3" t="n">
@@ -551,17 +551,17 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>['ABCAPITAL.NS', 'ABCAPITAL.BO']</t>
+          <t>[('ABCAPITAL', &lt;StockExchange.NSE: 'NSE'&gt;), ('ABCAPITAL', &lt;StockExchange.BSE: 'BSE'&gt;)]</t>
         </is>
       </c>
       <c r="F4" t="n">
-        <v>81.23125076293945</v>
+        <v>80.30000305175781</v>
       </c>
       <c r="G4" t="n">
-        <v>487.3875045776367</v>
+        <v>481.8000183105469</v>
       </c>
       <c r="H4" t="n">
-        <v>0.2316053946019448</v>
+        <v>0.2314343424310008</v>
       </c>
     </row>
     <row r="5">
@@ -581,17 +581,17 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>['BLACKROSE.BO']</t>
+          <t>[('BLACKROSE', &lt;StockExchange.BSE: 'BSE'&gt;)]</t>
         </is>
       </c>
       <c r="F5" t="n">
-        <v>80.85000133514404</v>
+        <v>80</v>
       </c>
       <c r="G5" t="n">
-        <v>1617.000026702881</v>
+        <v>1600</v>
       </c>
       <c r="H5" t="n">
-        <v>0.7683946053980552</v>
+        <v>0.7685656575689992</v>
       </c>
     </row>
     <row r="6">
@@ -611,7 +611,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>['ABCAPITAL.NS', 'ABCAPITAL.BO']</t>
+          <t>[('ABCAPITAL', &lt;StockExchange.NSE: 'NSE'&gt;), ('ABCAPITAL', &lt;StockExchange.BSE: 'BSE'&gt;)]</t>
         </is>
       </c>
       <c r="F6" t="n">
@@ -641,7 +641,7 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>['BLACKROSE.BO']</t>
+          <t>[('BLACKROSE', &lt;StockExchange.BSE: 'BSE'&gt;)]</t>
         </is>
       </c>
       <c r="F7" t="n">
@@ -671,7 +671,7 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>['ABCAPITAL.NS', 'ABCAPITAL.BO']</t>
+          <t>[('ABCAPITAL', &lt;StockExchange.NSE: 'NSE'&gt;), ('ABCAPITAL', &lt;StockExchange.BSE: 'BSE'&gt;)]</t>
         </is>
       </c>
       <c r="F8" t="n">
@@ -701,7 +701,7 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>['BLACKROSE.BO']</t>
+          <t>[('BLACKROSE', &lt;StockExchange.BSE: 'BSE'&gt;)]</t>
         </is>
       </c>
       <c r="F9" t="n">
@@ -731,7 +731,7 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>['ABCAPITAL.NS', 'ABCAPITAL.BO']</t>
+          <t>[('ABCAPITAL', &lt;StockExchange.NSE: 'NSE'&gt;), ('ABCAPITAL', &lt;StockExchange.BSE: 'BSE'&gt;)]</t>
         </is>
       </c>
       <c r="F10" t="n">
@@ -761,7 +761,7 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>['BLACKROSE.BO']</t>
+          <t>[('BLACKROSE', &lt;StockExchange.BSE: 'BSE'&gt;)]</t>
         </is>
       </c>
       <c r="F11" t="n">
@@ -791,7 +791,7 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>['ABCAPITAL.NS', 'ABCAPITAL.BO']</t>
+          <t>[('ABCAPITAL', &lt;StockExchange.NSE: 'NSE'&gt;), ('ABCAPITAL', &lt;StockExchange.BSE: 'BSE'&gt;)]</t>
         </is>
       </c>
       <c r="F12" t="n">
@@ -821,7 +821,7 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>['ABCAPITAL.NS', 'ABCAPITAL.BO']</t>
+          <t>[('ABCAPITAL', &lt;StockExchange.NSE: 'NSE'&gt;), ('ABCAPITAL', &lt;StockExchange.BSE: 'BSE'&gt;)]</t>
         </is>
       </c>
       <c r="F13" t="n">
@@ -851,7 +851,7 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>['BLACKROSE.BO']</t>
+          <t>[('BLACKROSE', &lt;StockExchange.BSE: 'BSE'&gt;)]</t>
         </is>
       </c>
       <c r="F14" t="n">
@@ -881,7 +881,7 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>['ABCAPITAL.NS', 'ABCAPITAL.BO']</t>
+          <t>[('ABCAPITAL', &lt;StockExchange.NSE: 'NSE'&gt;), ('ABCAPITAL', &lt;StockExchange.BSE: 'BSE'&gt;)]</t>
         </is>
       </c>
       <c r="F15" t="n">
@@ -911,7 +911,7 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>['BLACKROSE.BO']</t>
+          <t>[('BLACKROSE', &lt;StockExchange.BSE: 'BSE'&gt;)]</t>
         </is>
       </c>
       <c r="F16" t="n">
@@ -941,7 +941,7 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>['MON100.NS', 'MON100.BO']</t>
+          <t>[('MON100', &lt;StockExchange.NSE: 'NSE'&gt;), ('MON100', &lt;StockExchange.BSE: 'BSE'&gt;)]</t>
         </is>
       </c>
       <c r="F17" t="n">
@@ -971,7 +971,7 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>['ABCAPITAL.NS', 'ABCAPITAL.BO']</t>
+          <t>[('ABCAPITAL', &lt;StockExchange.NSE: 'NSE'&gt;), ('ABCAPITAL', &lt;StockExchange.BSE: 'BSE'&gt;)]</t>
         </is>
       </c>
       <c r="F18" t="n">
@@ -1001,7 +1001,7 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>['BLACKROSE.BO']</t>
+          <t>[('BLACKROSE', &lt;StockExchange.BSE: 'BSE'&gt;)]</t>
         </is>
       </c>
       <c r="F19" t="n">
@@ -1031,7 +1031,7 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>['MON100.NS', 'MON100.BO']</t>
+          <t>[('MON100', &lt;StockExchange.NSE: 'NSE'&gt;), ('MON100', &lt;StockExchange.BSE: 'BSE'&gt;)]</t>
         </is>
       </c>
       <c r="F20" t="n">
@@ -1061,7 +1061,7 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>['SAFARI.NS', 'SAFARIND.BO']</t>
+          <t>[('SAFARI', &lt;StockExchange.NSE: 'NSE'&gt;), ('SAFARIND', &lt;StockExchange.BSE: 'BSE'&gt;)]</t>
         </is>
       </c>
       <c r="F21" t="n">
@@ -1091,7 +1091,7 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>['ABCAPITAL.NS', 'ABCAPITAL.BO']</t>
+          <t>[('ABCAPITAL', &lt;StockExchange.NSE: 'NSE'&gt;), ('ABCAPITAL', &lt;StockExchange.BSE: 'BSE'&gt;)]</t>
         </is>
       </c>
       <c r="F22" t="n">
@@ -1121,7 +1121,7 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>['BLACKROSE.BO']</t>
+          <t>[('BLACKROSE', &lt;StockExchange.BSE: 'BSE'&gt;)]</t>
         </is>
       </c>
       <c r="F23" t="n">
@@ -1151,7 +1151,7 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>['MON100.NS', 'MON100.BO']</t>
+          <t>[('MON100', &lt;StockExchange.NSE: 'NSE'&gt;), ('MON100', &lt;StockExchange.BSE: 'BSE'&gt;)]</t>
         </is>
       </c>
       <c r="F24" t="n">
@@ -1181,7 +1181,7 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>['SAFARI.NS', 'SAFARIND.BO']</t>
+          <t>[('SAFARI', &lt;StockExchange.NSE: 'NSE'&gt;), ('SAFARIND', &lt;StockExchange.BSE: 'BSE'&gt;)]</t>
         </is>
       </c>
       <c r="F25" t="n">
@@ -1211,7 +1211,7 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>['ABCAPITAL.NS', 'ABCAPITAL.BO']</t>
+          <t>[('ABCAPITAL', &lt;StockExchange.NSE: 'NSE'&gt;), ('ABCAPITAL', &lt;StockExchange.BSE: 'BSE'&gt;)]</t>
         </is>
       </c>
       <c r="F26" t="n">
@@ -1241,7 +1241,7 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>['BLACKROSE.BO']</t>
+          <t>[('BLACKROSE', &lt;StockExchange.BSE: 'BSE'&gt;)]</t>
         </is>
       </c>
       <c r="F27" t="n">
@@ -1271,7 +1271,7 @@
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>['MON100.NS', 'MON100.BO']</t>
+          <t>[('MON100', &lt;StockExchange.NSE: 'NSE'&gt;), ('MON100', &lt;StockExchange.BSE: 'BSE'&gt;)]</t>
         </is>
       </c>
       <c r="F28" t="n">
@@ -1301,7 +1301,7 @@
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>['SAFARI.NS', 'SAFARIND.BO']</t>
+          <t>[('SAFARI', &lt;StockExchange.NSE: 'NSE'&gt;), ('SAFARIND', &lt;StockExchange.BSE: 'BSE'&gt;)]</t>
         </is>
       </c>
       <c r="F29" t="n">
@@ -1331,7 +1331,7 @@
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>['ABCAPITAL.NS', 'ABCAPITAL.BO']</t>
+          <t>[('ABCAPITAL', &lt;StockExchange.NSE: 'NSE'&gt;), ('ABCAPITAL', &lt;StockExchange.BSE: 'BSE'&gt;)]</t>
         </is>
       </c>
       <c r="F30" t="n">
@@ -1361,7 +1361,7 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>['BLACKROSE.BO']</t>
+          <t>[('BLACKROSE', &lt;StockExchange.BSE: 'BSE'&gt;)]</t>
         </is>
       </c>
       <c r="F31" t="n">
@@ -1391,7 +1391,7 @@
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>['MON100.NS', 'MON100.BO']</t>
+          <t>[('MON100', &lt;StockExchange.NSE: 'NSE'&gt;), ('MON100', &lt;StockExchange.BSE: 'BSE'&gt;)]</t>
         </is>
       </c>
       <c r="F32" t="n">
@@ -1421,7 +1421,7 @@
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>['SAFARI.NS', 'SAFARIND.BO']</t>
+          <t>[('SAFARI', &lt;StockExchange.NSE: 'NSE'&gt;), ('SAFARIND', &lt;StockExchange.BSE: 'BSE'&gt;)]</t>
         </is>
       </c>
       <c r="F33" t="n">
@@ -1451,7 +1451,7 @@
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>['ABCAPITAL.NS', 'ABCAPITAL.BO']</t>
+          <t>[('ABCAPITAL', &lt;StockExchange.NSE: 'NSE'&gt;), ('ABCAPITAL', &lt;StockExchange.BSE: 'BSE'&gt;)]</t>
         </is>
       </c>
       <c r="F34" t="n">
@@ -1481,7 +1481,7 @@
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>['MON100.NS', 'MON100.BO']</t>
+          <t>[('MON100', &lt;StockExchange.NSE: 'NSE'&gt;), ('MON100', &lt;StockExchange.BSE: 'BSE'&gt;)]</t>
         </is>
       </c>
       <c r="F35" t="n">
@@ -1511,7 +1511,7 @@
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>['SAFARI.NS', 'SAFARIND.BO']</t>
+          <t>[('SAFARI', &lt;StockExchange.NSE: 'NSE'&gt;), ('SAFARIND', &lt;StockExchange.BSE: 'BSE'&gt;)]</t>
         </is>
       </c>
       <c r="F36" t="n">
@@ -1541,7 +1541,7 @@
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>['ABCAPITAL.NS', 'ABCAPITAL.BO']</t>
+          <t>[('ABCAPITAL', &lt;StockExchange.NSE: 'NSE'&gt;), ('ABCAPITAL', &lt;StockExchange.BSE: 'BSE'&gt;)]</t>
         </is>
       </c>
       <c r="F37" t="n">
@@ -1571,7 +1571,7 @@
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>['MON100.NS', 'MON100.BO']</t>
+          <t>[('MON100', &lt;StockExchange.NSE: 'NSE'&gt;), ('MON100', &lt;StockExchange.BSE: 'BSE'&gt;)]</t>
         </is>
       </c>
       <c r="F38" t="n">
@@ -1601,7 +1601,7 @@
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>['SAFARI.NS', 'SAFARIND.BO']</t>
+          <t>[('SAFARI', &lt;StockExchange.NSE: 'NSE'&gt;), ('SAFARIND', &lt;StockExchange.BSE: 'BSE'&gt;)]</t>
         </is>
       </c>
       <c r="F39" t="n">
@@ -1631,7 +1631,7 @@
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>['BLACKROSE.BO']</t>
+          <t>[('BLACKROSE', &lt;StockExchange.BSE: 'BSE'&gt;)]</t>
         </is>
       </c>
       <c r="F40" t="n">
@@ -1661,7 +1661,7 @@
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>['ABCAPITAL.NS', 'ABCAPITAL.BO']</t>
+          <t>[('ABCAPITAL', &lt;StockExchange.NSE: 'NSE'&gt;), ('ABCAPITAL', &lt;StockExchange.BSE: 'BSE'&gt;)]</t>
         </is>
       </c>
       <c r="F41" t="n">
@@ -1691,7 +1691,7 @@
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>['MON100.NS', 'MON100.BO']</t>
+          <t>[('MON100', &lt;StockExchange.NSE: 'NSE'&gt;), ('MON100', &lt;StockExchange.BSE: 'BSE'&gt;)]</t>
         </is>
       </c>
       <c r="F42" t="n">
@@ -1721,7 +1721,7 @@
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>['SAFARI.NS', 'SAFARIND.BO']</t>
+          <t>[('SAFARI', &lt;StockExchange.NSE: 'NSE'&gt;), ('SAFARIND', &lt;StockExchange.BSE: 'BSE'&gt;)]</t>
         </is>
       </c>
       <c r="F43" t="n">
@@ -1751,7 +1751,7 @@
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>['BLACKROSE.BO']</t>
+          <t>[('BLACKROSE', &lt;StockExchange.BSE: 'BSE'&gt;)]</t>
         </is>
       </c>
       <c r="F44" t="n">
@@ -1781,7 +1781,7 @@
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>['ABCAPITAL.NS', 'ABCAPITAL.BO']</t>
+          <t>[('ABCAPITAL', &lt;StockExchange.NSE: 'NSE'&gt;), ('ABCAPITAL', &lt;StockExchange.BSE: 'BSE'&gt;)]</t>
         </is>
       </c>
       <c r="F45" t="n">
@@ -1811,7 +1811,7 @@
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>['MON100.NS', 'MON100.BO']</t>
+          <t>[('MON100', &lt;StockExchange.NSE: 'NSE'&gt;), ('MON100', &lt;StockExchange.BSE: 'BSE'&gt;)]</t>
         </is>
       </c>
       <c r="F46" t="n">
@@ -1841,7 +1841,7 @@
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>['SAFARI.NS', 'SAFARIND.BO']</t>
+          <t>[('SAFARI', &lt;StockExchange.NSE: 'NSE'&gt;), ('SAFARIND', &lt;StockExchange.BSE: 'BSE'&gt;)]</t>
         </is>
       </c>
       <c r="F47" t="n">
@@ -1871,7 +1871,7 @@
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>['BLACKROSE.BO']</t>
+          <t>[('BLACKROSE', &lt;StockExchange.BSE: 'BSE'&gt;)]</t>
         </is>
       </c>
       <c r="F48" t="n">
@@ -1901,7 +1901,7 @@
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>['ABCAPITAL.NS', 'ABCAPITAL.BO']</t>
+          <t>[('ABCAPITAL', &lt;StockExchange.NSE: 'NSE'&gt;), ('ABCAPITAL', &lt;StockExchange.BSE: 'BSE'&gt;)]</t>
         </is>
       </c>
       <c r="F49" t="n">
@@ -1931,7 +1931,7 @@
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>['MON100.NS', 'MON100.BO']</t>
+          <t>[('MON100', &lt;StockExchange.NSE: 'NSE'&gt;), ('MON100', &lt;StockExchange.BSE: 'BSE'&gt;)]</t>
         </is>
       </c>
       <c r="F50" t="n">
@@ -1961,7 +1961,7 @@
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>['SAFARI.NS', 'SAFARIND.BO']</t>
+          <t>[('SAFARI', &lt;StockExchange.NSE: 'NSE'&gt;), ('SAFARIND', &lt;StockExchange.BSE: 'BSE'&gt;)]</t>
         </is>
       </c>
       <c r="F51" t="n">
@@ -1991,7 +1991,7 @@
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>['BLACKROSE.BO']</t>
+          <t>[('BLACKROSE', &lt;StockExchange.BSE: 'BSE'&gt;)]</t>
         </is>
       </c>
       <c r="F52" t="n">
@@ -2021,7 +2021,7 @@
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>['ABCAPITAL.NS', 'ABCAPITAL.BO']</t>
+          <t>[('ABCAPITAL', &lt;StockExchange.NSE: 'NSE'&gt;), ('ABCAPITAL', &lt;StockExchange.BSE: 'BSE'&gt;)]</t>
         </is>
       </c>
       <c r="F53" t="n">
@@ -2051,7 +2051,7 @@
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>['MON100.NS', 'MON100.BO']</t>
+          <t>[('MON100', &lt;StockExchange.NSE: 'NSE'&gt;), ('MON100', &lt;StockExchange.BSE: 'BSE'&gt;)]</t>
         </is>
       </c>
       <c r="F54" t="n">
@@ -2081,7 +2081,7 @@
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>['SAFARI.NS', 'SAFARIND.BO']</t>
+          <t>[('SAFARI', &lt;StockExchange.NSE: 'NSE'&gt;), ('SAFARIND', &lt;StockExchange.BSE: 'BSE'&gt;)]</t>
         </is>
       </c>
       <c r="F55" t="n">
@@ -2111,7 +2111,7 @@
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>['BLACKROSE.BO']</t>
+          <t>[('BLACKROSE', &lt;StockExchange.BSE: 'BSE'&gt;)]</t>
         </is>
       </c>
       <c r="F56" t="n">

</xml_diff>